<commit_message>
binned and woe-replaced dataframe gen method added
</commit_message>
<xml_diff>
--- a/test_notebook/woe_t.xlsx
+++ b/test_notebook/woe_t.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>var_name</t>
   </si>
@@ -77,6 +77,15 @@
     <t>NumberOfDependents</t>
   </si>
   <si>
+    <t>test_cat1</t>
+  </si>
+  <si>
+    <t>test_cat2</t>
+  </si>
+  <si>
+    <t>test_U</t>
+  </si>
+  <si>
     <t>(-inf, 0.0192]</t>
   </si>
   <si>
@@ -107,13 +116,52 @@
     <t>(65.0, inf]</t>
   </si>
   <si>
-    <t>(-inf, 3.0]</t>
+    <t>(-inf, 0.0]</t>
+  </si>
+  <si>
+    <t>(0.0, inf]</t>
+  </si>
+  <si>
+    <t>(-inf, 0.134]</t>
+  </si>
+  <si>
+    <t>(0.134, 0.287]</t>
+  </si>
+  <si>
+    <t>(0.287, 0.468]</t>
+  </si>
+  <si>
+    <t>(0.468, 4.0]</t>
+  </si>
+  <si>
+    <t>(4.0, inf]</t>
+  </si>
+  <si>
+    <t>(-inf, 3000.0]</t>
+  </si>
+  <si>
+    <t>(3000.0, 4544.2]</t>
+  </si>
+  <si>
+    <t>(4544.2, 6300.0]</t>
+  </si>
+  <si>
+    <t>(6300.0, 9083.0]</t>
+  </si>
+  <si>
+    <t>(9083.0, inf]</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>(-inf, 4.0]</t>
   </si>
   <si>
     <t>(12.0, inf]</t>
   </si>
   <si>
-    <t>(3.0, 6.0]</t>
+    <t>(4.0, 6.0]</t>
   </si>
   <si>
     <t>(6.0, 9.0]</t>
@@ -122,60 +170,6 @@
     <t>(9.0, 12.0]</t>
   </si>
   <si>
-    <t>(-inf, 0.134]</t>
-  </si>
-  <si>
-    <t>(0.134, 0.287]</t>
-  </si>
-  <si>
-    <t>(0.287, 0.468]</t>
-  </si>
-  <si>
-    <t>(0.468, 4.0]</t>
-  </si>
-  <si>
-    <t>(4.0, inf]</t>
-  </si>
-  <si>
-    <t>(-inf, 3000.0]</t>
-  </si>
-  <si>
-    <t>(3000.0, 4544.2]</t>
-  </si>
-  <si>
-    <t>(4544.2, 6300.0]</t>
-  </si>
-  <si>
-    <t>(6300.0, 9083.0]</t>
-  </si>
-  <si>
-    <t>(9083.0, inf]</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>(-inf, 4.0]</t>
-  </si>
-  <si>
-    <t>(4.0, 6.0]</t>
-  </si>
-  <si>
-    <t>(-inf, 3.6]</t>
-  </si>
-  <si>
-    <t>(10.8, 14.4]</t>
-  </si>
-  <si>
-    <t>(14.4, inf]</t>
-  </si>
-  <si>
-    <t>(3.6, 7.2]</t>
-  </si>
-  <si>
-    <t>(7.2, 10.8]</t>
-  </si>
-  <si>
     <t>(-inf, 1.0]</t>
   </si>
   <si>
@@ -185,19 +179,37 @@
     <t>(2.0, inf]</t>
   </si>
   <si>
-    <t>(-inf, 2.4]</t>
-  </si>
-  <si>
-    <t>(10.2, inf]</t>
-  </si>
-  <si>
-    <t>(2.4, 4.8]</t>
-  </si>
-  <si>
-    <t>(4.8, 7.2]</t>
-  </si>
-  <si>
-    <t>(7.2, 10.2]</t>
+    <t>1_test</t>
+  </si>
+  <si>
+    <t>2_test</t>
+  </si>
+  <si>
+    <t>3_test</t>
+  </si>
+  <si>
+    <t>4_test</t>
+  </si>
+  <si>
+    <t>5_test</t>
+  </si>
+  <si>
+    <t>6_test</t>
+  </si>
+  <si>
+    <t>7_test</t>
+  </si>
+  <si>
+    <t>8_test</t>
+  </si>
+  <si>
+    <t>9_test</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>iv</t>
@@ -558,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -601,7 +613,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C2">
         <v>30000</v>
@@ -633,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>30000</v>
@@ -665,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>30000</v>
@@ -697,7 +709,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>30000</v>
@@ -729,7 +741,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>30000</v>
@@ -761,7 +773,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>32004</v>
@@ -793,7 +805,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>30540</v>
@@ -825,7 +837,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>29040</v>
@@ -857,7 +869,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>29817</v>
@@ -889,7 +901,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>28599</v>
@@ -921,31 +933,31 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12">
-        <v>148403</v>
+        <v>126018</v>
       </c>
       <c r="D12">
-        <v>9287</v>
+        <v>5041</v>
       </c>
       <c r="E12">
-        <v>139116</v>
+        <v>120977</v>
       </c>
       <c r="F12">
-        <v>0.9938702901967508</v>
+        <v>0.8642819380742138</v>
       </c>
       <c r="G12">
         <v>0.06684</v>
       </c>
       <c r="H12">
-        <v>0.9262916417314981</v>
+        <v>0.5027927388789148</v>
       </c>
       <c r="I12">
-        <v>-0.07041757244714834</v>
+        <v>-0.5417209975483785</v>
       </c>
       <c r="J12">
-        <v>0.004758724374182298</v>
+        <v>0.1958262895910419</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -953,127 +965,127 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C13">
-        <v>270</v>
+        <v>23982</v>
       </c>
       <c r="D13">
-        <v>148</v>
+        <v>4985</v>
       </c>
       <c r="E13">
-        <v>122</v>
+        <v>18997</v>
       </c>
       <c r="F13">
-        <v>0.0008715904382242416</v>
+        <v>0.1357180619257862</v>
       </c>
       <c r="G13">
         <v>0.06684</v>
       </c>
       <c r="H13">
-        <v>0.01476161978854977</v>
+        <v>0.4972072611210852</v>
       </c>
       <c r="I13">
-        <v>2.829466201266104</v>
+        <v>1.298427303686134</v>
       </c>
       <c r="J13">
-        <v>0.03930136858134026</v>
+        <v>0.469367446222812</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C14">
-        <v>1229</v>
+        <v>30000</v>
       </c>
       <c r="D14">
-        <v>546</v>
+        <v>1830</v>
       </c>
       <c r="E14">
-        <v>683</v>
+        <v>28170</v>
       </c>
       <c r="F14">
-        <v>0.004879477617271779</v>
+        <v>0.2012516610227614</v>
       </c>
       <c r="G14">
         <v>0.06684</v>
       </c>
       <c r="H14">
-        <v>0.05445840813883902</v>
+        <v>0.182525433871933</v>
       </c>
       <c r="I14">
-        <v>2.41239908840936</v>
+        <v>-0.09766664279970659</v>
       </c>
       <c r="J14">
-        <v>0.1196041667945398</v>
+        <v>0.001828927738126124</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C15">
-        <v>91</v>
+        <v>30000</v>
       </c>
       <c r="D15">
-        <v>40</v>
+        <v>1716</v>
       </c>
       <c r="E15">
-        <v>51</v>
+        <v>28284</v>
       </c>
       <c r="F15">
-        <v>0.0003643533799134125</v>
+        <v>0.2020660979896267</v>
       </c>
       <c r="G15">
         <v>0.06684</v>
       </c>
       <c r="H15">
-        <v>0.003989626969878316</v>
+        <v>0.1711549970077798</v>
       </c>
       <c r="I15">
-        <v>2.393328793624856</v>
+        <v>-0.1660253004409788</v>
       </c>
       <c r="J15">
-        <v>0.008676471667630753</v>
+        <v>0.005132024827472562</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>30000</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>1853</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>28147</v>
       </c>
       <c r="F16">
-        <v>1.428836783974167e-05</v>
+        <v>0.2010873447926043</v>
       </c>
       <c r="G16">
         <v>0.06684</v>
       </c>
       <c r="H16">
-        <v>0.0004987033712347895</v>
+        <v>0.184819469379613</v>
       </c>
       <c r="I16">
-        <v>3.5525657041094</v>
+        <v>-0.08435985743198259</v>
       </c>
       <c r="J16">
-        <v>0.001720916127617286</v>
+        <v>0.001372355650561205</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1081,31 +1093,31 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C17">
-        <v>30000</v>
+        <v>30109</v>
       </c>
       <c r="D17">
-        <v>1830</v>
+        <v>2974</v>
       </c>
       <c r="E17">
-        <v>28170</v>
+        <v>27135</v>
       </c>
       <c r="F17">
-        <v>0.2012516610227614</v>
+        <v>0.1938574306656951</v>
       </c>
       <c r="G17">
         <v>0.06684</v>
       </c>
       <c r="H17">
-        <v>0.182525433871933</v>
+        <v>0.2966287652104528</v>
       </c>
       <c r="I17">
-        <v>-0.09766664279970659</v>
+        <v>0.4253584127578403</v>
       </c>
       <c r="J17">
-        <v>0.001828927738126124</v>
+        <v>0.04371465173896318</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1113,127 +1125,127 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C18">
-        <v>30000</v>
+        <v>29891</v>
       </c>
       <c r="D18">
-        <v>1716</v>
+        <v>1653</v>
       </c>
       <c r="E18">
-        <v>28284</v>
+        <v>28238</v>
       </c>
       <c r="F18">
-        <v>0.2020660979896267</v>
+        <v>0.2017374655293126</v>
       </c>
       <c r="G18">
         <v>0.06684</v>
       </c>
       <c r="H18">
-        <v>0.1711549970077798</v>
+        <v>0.1648713345302214</v>
       </c>
       <c r="I18">
-        <v>-0.1660253004409788</v>
+        <v>-0.2018017975132012</v>
       </c>
       <c r="J18">
-        <v>0.005132024827472562</v>
+        <v>0.007439651502973746</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>30000</v>
+        <v>25084</v>
       </c>
       <c r="D19">
-        <v>1853</v>
+        <v>2277</v>
       </c>
       <c r="E19">
-        <v>28147</v>
+        <v>22807</v>
       </c>
       <c r="F19">
-        <v>0.2010873447926043</v>
+        <v>0.1629374026604941</v>
       </c>
       <c r="G19">
         <v>0.06684</v>
       </c>
       <c r="H19">
-        <v>0.184819469379613</v>
+        <v>0.2271095152603232</v>
       </c>
       <c r="I19">
-        <v>-0.08435985743198259</v>
+        <v>0.3320662529328347</v>
       </c>
       <c r="J19">
-        <v>0.001372355650561205</v>
+        <v>0.02130939297380919</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C20">
-        <v>30109</v>
+        <v>23024</v>
       </c>
       <c r="D20">
-        <v>2974</v>
+        <v>1979</v>
       </c>
       <c r="E20">
-        <v>27135</v>
+        <v>21045</v>
       </c>
       <c r="F20">
-        <v>0.1938574306656951</v>
+        <v>0.1503493505936817</v>
       </c>
       <c r="G20">
         <v>0.06684</v>
       </c>
       <c r="H20">
-        <v>0.2966287652104528</v>
+        <v>0.1973867943347297</v>
       </c>
       <c r="I20">
-        <v>0.4253584127578403</v>
+        <v>0.2722036366331397</v>
       </c>
       <c r="J20">
-        <v>0.04371465173896318</v>
+        <v>0.01280376324423999</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>29891</v>
+        <v>24057</v>
       </c>
       <c r="D21">
-        <v>1653</v>
+        <v>1687</v>
       </c>
       <c r="E21">
-        <v>28238</v>
+        <v>22370</v>
       </c>
       <c r="F21">
-        <v>0.2017374655293126</v>
+        <v>0.1598153942875105</v>
       </c>
       <c r="G21">
         <v>0.06684</v>
       </c>
       <c r="H21">
-        <v>0.1648713345302214</v>
+        <v>0.168262517454618</v>
       </c>
       <c r="I21">
-        <v>-0.2018017975132012</v>
+        <v>0.05150600029703796</v>
       </c>
       <c r="J21">
-        <v>0.007439651502973746</v>
+        <v>0.000435077528354152</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1241,31 +1253,31 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>25084</v>
+        <v>24084</v>
       </c>
       <c r="D22">
-        <v>2277</v>
+        <v>1332</v>
       </c>
       <c r="E22">
-        <v>22807</v>
+        <v>22752</v>
       </c>
       <c r="F22">
-        <v>0.1629374026604941</v>
+        <v>0.1625444725449012</v>
       </c>
       <c r="G22">
         <v>0.06684</v>
       </c>
       <c r="H22">
-        <v>0.2271095152603232</v>
+        <v>0.1328545780969479</v>
       </c>
       <c r="I22">
-        <v>0.3320662529328347</v>
+        <v>-0.2016965092673882</v>
       </c>
       <c r="J22">
-        <v>0.02130939297380919</v>
+        <v>0.005988348070669385</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1273,31 +1285,31 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C23">
-        <v>23024</v>
+        <v>24020</v>
       </c>
       <c r="D23">
-        <v>1979</v>
+        <v>1082</v>
       </c>
       <c r="E23">
-        <v>21045</v>
+        <v>22938</v>
       </c>
       <c r="F23">
-        <v>0.1503493505936817</v>
+        <v>0.1638732907539972</v>
       </c>
       <c r="G23">
         <v>0.06684</v>
       </c>
       <c r="H23">
-        <v>0.1973867943347297</v>
+        <v>0.1079194095352085</v>
       </c>
       <c r="I23">
-        <v>0.2722036366331397</v>
+        <v>-0.417708771282796</v>
       </c>
       <c r="J23">
-        <v>0.01280376324423999</v>
+        <v>0.02337242697240375</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1305,127 +1317,127 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C24">
-        <v>24057</v>
+        <v>29731</v>
       </c>
       <c r="D24">
-        <v>1687</v>
+        <v>1669</v>
       </c>
       <c r="E24">
-        <v>22370</v>
+        <v>28062</v>
       </c>
       <c r="F24">
-        <v>0.1598153942875105</v>
+        <v>0.2004800891594153</v>
       </c>
       <c r="G24">
         <v>0.06684</v>
       </c>
       <c r="H24">
-        <v>0.168262517454618</v>
+        <v>0.1664671853181728</v>
       </c>
       <c r="I24">
-        <v>0.05150600029703796</v>
+        <v>-0.185916731056861</v>
       </c>
       <c r="J24">
-        <v>0.000435077528354152</v>
+        <v>0.006323567895915169</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C25">
-        <v>24084</v>
+        <v>33659</v>
       </c>
       <c r="D25">
-        <v>1332</v>
+        <v>3103</v>
       </c>
       <c r="E25">
-        <v>22752</v>
+        <v>30556</v>
       </c>
       <c r="F25">
-        <v>0.1625444725449012</v>
+        <v>0.2182976838555732</v>
       </c>
       <c r="G25">
         <v>0.06684</v>
       </c>
       <c r="H25">
-        <v>0.1328545780969479</v>
+        <v>0.3094953121883104</v>
       </c>
       <c r="I25">
-        <v>-0.2016965092673882</v>
+        <v>0.3490832920223748</v>
       </c>
       <c r="J25">
-        <v>0.005988348070669385</v>
+        <v>0.0318355683230249</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C26">
-        <v>24020</v>
+        <v>27684</v>
       </c>
       <c r="D26">
-        <v>1082</v>
+        <v>1846</v>
       </c>
       <c r="E26">
-        <v>22938</v>
+        <v>25838</v>
       </c>
       <c r="F26">
-        <v>0.1638732907539972</v>
+        <v>0.1845914241216226</v>
       </c>
       <c r="G26">
         <v>0.06684</v>
       </c>
       <c r="H26">
-        <v>0.1079194095352085</v>
+        <v>0.1841212846598843</v>
       </c>
       <c r="I26">
-        <v>-0.417708771282796</v>
+        <v>-0.002550168222204021</v>
       </c>
       <c r="J26">
-        <v>0.02337242697240375</v>
+        <v>1.198934715329032e-06</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C27">
-        <v>29731</v>
+        <v>26545</v>
       </c>
       <c r="D27">
-        <v>1669</v>
+        <v>1573</v>
       </c>
       <c r="E27">
-        <v>28062</v>
+        <v>24972</v>
       </c>
       <c r="F27">
-        <v>0.2004800891594153</v>
+        <v>0.1784045608470144</v>
       </c>
       <c r="G27">
         <v>0.06684</v>
       </c>
       <c r="H27">
-        <v>0.1664671853181728</v>
+        <v>0.1568920805904648</v>
       </c>
       <c r="I27">
-        <v>-0.185916731056861</v>
+        <v>-0.1284956008881118</v>
       </c>
       <c r="J27">
-        <v>0.006323567895915169</v>
+        <v>0.002764259077158989</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1433,31 +1445,31 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C28">
-        <v>33659</v>
+        <v>37162</v>
       </c>
       <c r="D28">
-        <v>3103</v>
+        <v>2017</v>
       </c>
       <c r="E28">
-        <v>30556</v>
+        <v>35145</v>
       </c>
       <c r="F28">
-        <v>0.2182976838555732</v>
+        <v>0.2510823438638604</v>
       </c>
       <c r="G28">
         <v>0.06684</v>
       </c>
       <c r="H28">
-        <v>0.3094953121883104</v>
+        <v>0.2011769399561141</v>
       </c>
       <c r="I28">
-        <v>0.3490832920223748</v>
+        <v>-0.2215961294205489</v>
       </c>
       <c r="J28">
-        <v>0.0318355683230249</v>
+        <v>0.01105884434312572</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1465,671 +1477,927 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C29">
-        <v>27684</v>
+        <v>24950</v>
       </c>
       <c r="D29">
-        <v>1846</v>
+        <v>1487</v>
       </c>
       <c r="E29">
-        <v>25838</v>
+        <v>23463</v>
       </c>
       <c r="F29">
-        <v>0.1845914241216226</v>
+        <v>0.1676239873119293</v>
       </c>
       <c r="G29">
         <v>0.06684</v>
       </c>
       <c r="H29">
-        <v>0.1841212846598843</v>
+        <v>0.1483143826052264</v>
       </c>
       <c r="I29">
-        <v>-0.002550168222204021</v>
+        <v>-0.1223890725743209</v>
       </c>
       <c r="J29">
-        <v>1.198934715329032e-06</v>
+        <v>0.002363284611830114</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C30">
-        <v>26545</v>
+        <v>141662</v>
       </c>
       <c r="D30">
-        <v>1573</v>
+        <v>6554</v>
       </c>
       <c r="E30">
-        <v>24972</v>
+        <v>135108</v>
       </c>
       <c r="F30">
-        <v>0.1784045608470144</v>
+        <v>0.9652364010459086</v>
       </c>
       <c r="G30">
         <v>0.06684</v>
       </c>
       <c r="H30">
-        <v>0.1568920805904648</v>
+        <v>0.6537003790145621</v>
       </c>
       <c r="I30">
-        <v>-0.1284956008881118</v>
+        <v>-0.3897239360971259</v>
       </c>
       <c r="J30">
-        <v>0.002764259077158989</v>
+        <v>0.1214130447420973</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C31">
-        <v>37162</v>
+        <v>8338</v>
       </c>
       <c r="D31">
-        <v>2017</v>
+        <v>3472</v>
       </c>
       <c r="E31">
-        <v>35145</v>
+        <v>4866</v>
       </c>
       <c r="F31">
-        <v>0.2510823438638604</v>
+        <v>0.03476359895409147</v>
       </c>
       <c r="G31">
         <v>0.06684</v>
       </c>
       <c r="H31">
-        <v>0.2011769399561141</v>
+        <v>0.3462996209854379</v>
       </c>
       <c r="I31">
-        <v>-0.2215961294205489</v>
+        <v>2.298733524672018</v>
       </c>
       <c r="J31">
-        <v>0.01105884434312572</v>
+        <v>0.7161382979864164</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C32">
-        <v>24950</v>
+        <v>108526</v>
       </c>
       <c r="D32">
-        <v>1487</v>
+        <v>7420</v>
       </c>
       <c r="E32">
-        <v>23463</v>
+        <v>101106</v>
       </c>
       <c r="F32">
-        <v>0.1676239873119293</v>
+        <v>0.7223198594024605</v>
       </c>
       <c r="G32">
         <v>0.06684</v>
       </c>
       <c r="H32">
-        <v>0.1483143826052264</v>
+        <v>0.7400758029124277</v>
       </c>
       <c r="I32">
-        <v>-0.1223890725743209</v>
+        <v>0.02428455796807364</v>
       </c>
       <c r="J32">
-        <v>0.002363284611830114</v>
+        <v>0.0004311952394456401</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C33">
-        <v>149127</v>
+        <v>31522</v>
       </c>
       <c r="D33">
-        <v>9480</v>
+        <v>1765</v>
       </c>
       <c r="E33">
-        <v>139647</v>
+        <v>29757</v>
       </c>
       <c r="F33">
-        <v>0.9976638518582023</v>
+        <v>0.2125894809035964</v>
       </c>
       <c r="G33">
         <v>0.06684</v>
       </c>
       <c r="H33">
-        <v>0.9455415918611609</v>
+        <v>0.1760422900458807</v>
       </c>
       <c r="I33">
-        <v>-0.05365852138114158</v>
+        <v>-0.1886387358114613</v>
       </c>
       <c r="J33">
-        <v>0.002796803402484664</v>
+        <v>0.006894215880859683</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C34">
-        <v>13</v>
+        <v>9952</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>841</v>
       </c>
       <c r="E34">
-        <v>6</v>
+        <v>9111</v>
       </c>
       <c r="F34">
-        <v>4.2865103519225e-05</v>
+        <v>0.06509065969394316</v>
       </c>
       <c r="G34">
         <v>0.06684</v>
       </c>
       <c r="H34">
-        <v>0.0006981847197287054</v>
+        <v>0.0838819070416916</v>
       </c>
       <c r="I34">
-        <v>2.790425652062503</v>
+        <v>0.2536288784943346</v>
       </c>
       <c r="J34">
-        <v>0.001828620667370689</v>
+        <v>0.004766002990319077</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C35">
-        <v>272</v>
+        <v>142396</v>
       </c>
       <c r="D35">
-        <v>148</v>
+        <v>7256</v>
       </c>
       <c r="E35">
-        <v>124</v>
+        <v>135140</v>
       </c>
       <c r="F35">
-        <v>0.0008858788060639833</v>
+        <v>0.9654650149313444</v>
       </c>
       <c r="G35">
         <v>0.06684</v>
       </c>
       <c r="H35">
-        <v>0.01476161978854977</v>
+        <v>0.7237183323359266</v>
       </c>
       <c r="I35">
-        <v>2.813205680394323</v>
+        <v>-0.2882075930759481</v>
       </c>
       <c r="J35">
-        <v>0.03903531335160933</v>
+        <v>0.06967322952492054</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C36">
-        <v>540</v>
+        <v>7604</v>
       </c>
       <c r="D36">
-        <v>357</v>
+        <v>2770</v>
       </c>
       <c r="E36">
-        <v>183</v>
+        <v>4834</v>
       </c>
       <c r="F36">
-        <v>0.001307385657336363</v>
+        <v>0.03453498506865561</v>
       </c>
       <c r="G36">
         <v>0.06684</v>
       </c>
       <c r="H36">
-        <v>0.03560742070616398</v>
+        <v>0.2762816676640734</v>
       </c>
       <c r="I36">
-        <v>3.304524601173463</v>
+        <v>2.079448010153201</v>
       </c>
       <c r="J36">
-        <v>0.1133453096399629</v>
+        <v>0.5026996580841789</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37">
-        <v>48</v>
+        <v>113218</v>
       </c>
       <c r="D37">
-        <v>34</v>
+        <v>7030</v>
       </c>
       <c r="E37">
-        <v>14</v>
+        <v>106188</v>
       </c>
       <c r="F37">
-        <v>0.0001000185748781917</v>
+        <v>0.7586266020832441</v>
       </c>
       <c r="G37">
         <v>0.06684</v>
       </c>
       <c r="H37">
-        <v>0.003391182924396569</v>
+        <v>0.7011769399561141</v>
       </c>
       <c r="I37">
-        <v>3.523578167236148</v>
+        <v>-0.07874943001539493</v>
       </c>
       <c r="J37">
-        <v>0.01159667484674891</v>
+        <v>0.004524128147088508</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38">
-        <v>108526</v>
+        <v>19522</v>
       </c>
       <c r="D38">
-        <v>7420</v>
+        <v>1584</v>
       </c>
       <c r="E38">
-        <v>101106</v>
+        <v>17938</v>
       </c>
       <c r="F38">
-        <v>0.7223198594024605</v>
+        <v>0.128152371154643</v>
       </c>
       <c r="G38">
         <v>0.06684</v>
       </c>
       <c r="H38">
-        <v>0.7400758029124277</v>
+        <v>0.1579892280071813</v>
       </c>
       <c r="I38">
-        <v>0.02428455796807364</v>
+        <v>0.2093068979316677</v>
       </c>
       <c r="J38">
-        <v>0.0004311952394456401</v>
+        <v>0.006245059951836016</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39">
-        <v>31522</v>
+        <v>13336</v>
       </c>
       <c r="D39">
-        <v>1765</v>
+        <v>1233</v>
       </c>
       <c r="E39">
-        <v>29757</v>
+        <v>12103</v>
       </c>
       <c r="F39">
-        <v>0.2125894809035964</v>
+        <v>0.0864660579821967</v>
       </c>
       <c r="G39">
         <v>0.06684</v>
       </c>
       <c r="H39">
-        <v>0.1760422900458807</v>
+        <v>0.1229802513464991</v>
       </c>
       <c r="I39">
-        <v>-0.1886387358114613</v>
+        <v>0.3522718406609855</v>
       </c>
       <c r="J39">
-        <v>0.006894215880859683</v>
+        <v>0.01286292210669395</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C40">
-        <v>9952</v>
+        <v>3924</v>
       </c>
       <c r="D40">
-        <v>841</v>
+        <v>179</v>
       </c>
       <c r="E40">
-        <v>9111</v>
+        <v>3745</v>
       </c>
       <c r="F40">
-        <v>0.06509065969394316</v>
+        <v>0.02675496877991627</v>
       </c>
       <c r="G40">
         <v>0.06684</v>
       </c>
       <c r="H40">
-        <v>0.0838819070416916</v>
+        <v>0.01785358069020547</v>
       </c>
       <c r="I40">
-        <v>0.2536288784943346</v>
+        <v>-0.4045161178753199</v>
       </c>
       <c r="J40">
-        <v>0.004766002990319077</v>
+        <v>0.003600754953751425</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C41">
-        <v>149245</v>
+        <v>30086</v>
       </c>
       <c r="D41">
-        <v>9594</v>
+        <v>2023</v>
       </c>
       <c r="E41">
-        <v>139651</v>
+        <v>28063</v>
       </c>
       <c r="F41">
-        <v>0.9976924285938817</v>
+        <v>0.2004872333433352</v>
       </c>
       <c r="G41">
         <v>0.06684</v>
       </c>
       <c r="H41">
-        <v>0.9569120287253142</v>
+        <v>0.2017753840015959</v>
       </c>
       <c r="I41">
-        <v>-0.04173357780947094</v>
+        <v>0.006404547705170255</v>
       </c>
       <c r="J41">
-        <v>0.001701911991016201</v>
+        <v>8.250022342277016e-06</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C42">
-        <v>270</v>
+        <v>30215</v>
       </c>
       <c r="D42">
-        <v>148</v>
+        <v>2027</v>
       </c>
       <c r="E42">
-        <v>122</v>
+        <v>28188</v>
       </c>
       <c r="F42">
-        <v>0.0008715904382242416</v>
+        <v>0.201380256333319</v>
       </c>
       <c r="G42">
         <v>0.06684</v>
       </c>
       <c r="H42">
-        <v>0.01476161978854977</v>
+        <v>0.2021743466985837</v>
       </c>
       <c r="I42">
-        <v>2.829466201266104</v>
+        <v>0.003935484240331996</v>
       </c>
       <c r="J42">
-        <v>0.03930136858134026</v>
+        <v>3.125130117898505e-06</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C43">
-        <v>423</v>
+        <v>29876</v>
       </c>
       <c r="D43">
-        <v>245</v>
+        <v>2062</v>
       </c>
       <c r="E43">
-        <v>178</v>
+        <v>27814</v>
       </c>
       <c r="F43">
-        <v>0.001271664737737008</v>
+        <v>0.1987083315472873</v>
       </c>
       <c r="G43">
         <v>0.06684</v>
       </c>
       <c r="H43">
-        <v>0.02443646519050469</v>
+        <v>0.2056652702972272</v>
       </c>
       <c r="I43">
-        <v>2.955749632487887</v>
+        <v>0.03441186677359411</v>
       </c>
       <c r="J43">
-        <v>0.0684693504249233</v>
+        <v>0.0002394012494149847</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C44">
-        <v>59</v>
+        <v>29856</v>
       </c>
       <c r="D44">
-        <v>38</v>
+        <v>1966</v>
       </c>
       <c r="E44">
-        <v>21</v>
+        <v>27890</v>
       </c>
       <c r="F44">
-        <v>0.0001500278623172875</v>
+        <v>0.1992512895251976</v>
       </c>
       <c r="G44">
         <v>0.06684</v>
       </c>
       <c r="H44">
-        <v>0.003790145621384401</v>
+        <v>0.1960901655695192</v>
       </c>
       <c r="I44">
-        <v>3.229338694238208</v>
+        <v>-0.01599220767917783</v>
       </c>
       <c r="J44">
-        <v>0.0117551731309391</v>
+        <v>5.055335079883154e-05</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>29967</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>1948</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>28019</v>
       </c>
       <c r="F45">
-        <v>1.428836783974167e-05</v>
+        <v>0.2001728892508609</v>
       </c>
       <c r="G45">
         <v>0.06684</v>
       </c>
       <c r="H45">
-        <v>9.974067424695791e-05</v>
+        <v>0.194294833433074</v>
       </c>
       <c r="I45">
-        <v>1.9431277916753</v>
+        <v>-0.0298046740226936</v>
       </c>
       <c r="J45">
-        <v>0.0001660447514426152</v>
+        <v>0.000175193537536335</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C46">
-        <v>113218</v>
+        <v>15011</v>
       </c>
       <c r="D46">
-        <v>7030</v>
+        <v>967</v>
       </c>
       <c r="E46">
-        <v>106188</v>
+        <v>14044</v>
       </c>
       <c r="F46">
-        <v>0.7586266020832441</v>
+        <v>0.100332918970666</v>
       </c>
       <c r="G46">
         <v>0.06684</v>
       </c>
       <c r="H46">
-        <v>0.7011769399561141</v>
+        <v>0.0964492319968083</v>
       </c>
       <c r="I46">
-        <v>-0.07874943001539493</v>
+        <v>-0.03947706959978357</v>
       </c>
       <c r="J46">
-        <v>0.004524128147088508</v>
+        <v>0.0001533165809707527</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C47">
-        <v>19522</v>
+        <v>15019</v>
       </c>
       <c r="D47">
-        <v>1584</v>
+        <v>966</v>
       </c>
       <c r="E47">
-        <v>17938</v>
+        <v>14053</v>
       </c>
       <c r="F47">
-        <v>0.128152371154643</v>
+        <v>0.1003972166259448</v>
       </c>
       <c r="G47">
         <v>0.06684</v>
       </c>
       <c r="H47">
-        <v>0.1579892280071813</v>
+        <v>0.09634949132256133</v>
       </c>
       <c r="I47">
-        <v>0.2093068979316677</v>
+        <v>-0.0411523686529821</v>
       </c>
       <c r="J47">
-        <v>0.006245059951836016</v>
+        <v>0.0001665734838908411</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C48">
-        <v>13336</v>
+        <v>14907</v>
       </c>
       <c r="D48">
-        <v>1233</v>
+        <v>1037</v>
       </c>
       <c r="E48">
-        <v>12103</v>
+        <v>13870</v>
       </c>
       <c r="F48">
-        <v>0.0864660579821967</v>
+        <v>0.09908983096860846</v>
       </c>
       <c r="G48">
         <v>0.06684</v>
       </c>
       <c r="H48">
-        <v>0.1229802513464991</v>
+        <v>0.1034310791940953</v>
       </c>
       <c r="I48">
-        <v>0.3522718406609855</v>
+        <v>0.04287866715589498</v>
       </c>
       <c r="J48">
-        <v>0.01286292210669395</v>
+        <v>0.0001861469377017719</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49">
+        <v>15068</v>
+      </c>
+      <c r="D49">
+        <v>1010</v>
+      </c>
+      <c r="E49">
+        <v>14058</v>
+      </c>
+      <c r="F49">
+        <v>0.1004329375455442</v>
+      </c>
+      <c r="G49">
+        <v>0.06684</v>
+      </c>
+      <c r="H49">
+        <v>0.1007380809894275</v>
+      </c>
+      <c r="I49">
+        <v>0.003033674334699487</v>
+      </c>
+      <c r="J49">
+        <v>9.257058341106194e-07</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50">
+        <v>15084</v>
+      </c>
+      <c r="D50">
+        <v>1025</v>
+      </c>
+      <c r="E50">
+        <v>14059</v>
+      </c>
+      <c r="F50">
+        <v>0.100440081729464</v>
+      </c>
+      <c r="G50">
+        <v>0.06684</v>
+      </c>
+      <c r="H50">
+        <v>0.1022341911031319</v>
+      </c>
+      <c r="I50">
+        <v>0.01770482472784601</v>
+      </c>
+      <c r="J50">
+        <v>3.17643920033741e-05</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51">
+        <v>15007</v>
+      </c>
+      <c r="D51">
+        <v>1037</v>
+      </c>
+      <c r="E51">
+        <v>13970</v>
+      </c>
+      <c r="F51">
+        <v>0.09980424936059554</v>
+      </c>
+      <c r="G51">
+        <v>0.06684</v>
+      </c>
+      <c r="H51">
+        <v>0.1034310791940953</v>
+      </c>
+      <c r="I51">
+        <v>0.03569472821376486</v>
+      </c>
+      <c r="J51">
+        <v>0.0001294587051843497</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52">
+        <v>15055</v>
+      </c>
+      <c r="D52">
+        <v>947</v>
+      </c>
+      <c r="E52">
+        <v>14108</v>
+      </c>
+      <c r="F52">
+        <v>0.1007901467415377</v>
+      </c>
+      <c r="G52">
+        <v>0.06684</v>
+      </c>
+      <c r="H52">
+        <v>0.09445441851186914</v>
+      </c>
+      <c r="I52">
+        <v>-0.0649232259346193</v>
+      </c>
+      <c r="J52">
+        <v>0.0004113359153151184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53">
+        <v>14924</v>
+      </c>
+      <c r="D53">
+        <v>1032</v>
+      </c>
+      <c r="E53">
+        <v>13892</v>
+      </c>
+      <c r="F53">
+        <v>0.09924700301484561</v>
+      </c>
+      <c r="G53">
+        <v>0.06684</v>
+      </c>
+      <c r="H53">
+        <v>0.1029323758228606</v>
+      </c>
+      <c r="I53">
+        <v>0.03646050441278845</v>
+      </c>
+      <c r="J53">
+        <v>0.0001343705515293997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54">
+        <v>14933</v>
+      </c>
+      <c r="D54">
+        <v>975</v>
+      </c>
+      <c r="E54">
+        <v>13958</v>
+      </c>
+      <c r="F54">
+        <v>0.09971851915355709</v>
+      </c>
+      <c r="G54">
+        <v>0.06684</v>
+      </c>
+      <c r="H54">
+        <v>0.09724715739078396</v>
+      </c>
+      <c r="I54">
+        <v>-0.02509565634400479</v>
+      </c>
+      <c r="J54">
+        <v>6.20204455002683e-05</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" t="s">
         <v>45</v>
       </c>
-      <c r="C49">
-        <v>3924</v>
-      </c>
-      <c r="D49">
-        <v>179</v>
-      </c>
-      <c r="E49">
-        <v>3745</v>
-      </c>
-      <c r="F49">
-        <v>0.02675496877991627</v>
-      </c>
-      <c r="G49">
-        <v>0.06684</v>
-      </c>
-      <c r="H49">
-        <v>0.01785358069020547</v>
-      </c>
-      <c r="I49">
-        <v>-0.4045161178753199</v>
-      </c>
-      <c r="J49">
-        <v>0.003600754953751425</v>
+      <c r="C55">
+        <v>14992</v>
+      </c>
+      <c r="D55">
+        <v>1030</v>
+      </c>
+      <c r="E55">
+        <v>13962</v>
+      </c>
+      <c r="F55">
+        <v>0.09974709588923657</v>
+      </c>
+      <c r="G55">
+        <v>0.06684</v>
+      </c>
+      <c r="H55">
+        <v>0.1027328944743666</v>
+      </c>
+      <c r="I55">
+        <v>0.02949442092857983</v>
+      </c>
+      <c r="J55">
+        <v>8.806440027778473e-05</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56">
+        <v>139974</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>139974</v>
+      </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>0.06684</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>-10</v>
+      </c>
+      <c r="J56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57">
+        <v>10026</v>
+      </c>
+      <c r="D57">
+        <v>10026</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0.06684</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>10</v>
+      </c>
+      <c r="J57">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2139,7 +2407,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2150,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2190,7 +2458,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>0.1740616475453104</v>
+        <v>0.6651937358138539</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2198,7 +2466,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0.1213938488796615</v>
+        <v>0.5723728876090994</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2206,7 +2474,7 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.1686027219081765</v>
+        <v>0.8375513427285136</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2231,6 +2499,30 @@
       </c>
       <c r="B11">
         <v>0.2500393230671014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>0.0004765232902103267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>0.001363977118207771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>